<commit_message>
Updated test synthesis and convergence table
</commit_message>
<xml_diff>
--- a/tests/validation/test_synthesis/Convergence_table_short.xlsx
+++ b/tests/validation/test_synthesis/Convergence_table_short.xlsx
@@ -14,14 +14,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="35">
   <si>
     <t>PDE_model</t>
   </si>
   <si>
-    <t>Numerical_method_space_discretization</t>
-  </si>
-  <si>
     <t>Numerical_method_name</t>
   </si>
   <si>
@@ -37,13 +34,43 @@
     <t>Mesh_cell_type</t>
   </si>
   <si>
-    <t>Color</t>
+    <t>Test_color</t>
+  </si>
+  <si>
+    <t>Computational_time</t>
+  </si>
+  <si>
+    <t>Wave system</t>
+  </si>
+  <si>
+    <t>Upwind</t>
+  </si>
+  <si>
+    <t>Deformed quadrangles</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>Regular brick wall</t>
+  </si>
+  <si>
+    <t>Squares</t>
   </si>
   <si>
     <t>Poisson</t>
   </si>
   <si>
-    <t>Finite elements</t>
+    <t>VF5</t>
+  </si>
+  <si>
+    <t>Regular hexagons</t>
+  </si>
+  <si>
+    <t>Unstructured triangles</t>
+  </si>
+  <si>
+    <t>Triangles</t>
   </si>
   <si>
     <t>P1 FE</t>
@@ -52,46 +79,46 @@
     <t>Unstructured 3D triangles</t>
   </si>
   <si>
+    <t>3DTriangles</t>
+  </si>
+  <si>
+    <t>Regular squares</t>
+  </si>
+  <si>
+    <t>Regular tetrahedra</t>
+  </si>
+  <si>
     <t>Tetrahedra</t>
   </si>
   <si>
-    <t>Green</t>
-  </si>
-  <si>
-    <t>Finite volumes</t>
-  </si>
-  <si>
-    <t>VF5</t>
-  </si>
-  <si>
     <t>Non conforming cartesian locally refined</t>
   </si>
   <si>
-    <t>Squares</t>
-  </si>
-  <si>
-    <t>Unstructured triangles</t>
-  </si>
-  <si>
-    <t>Triangles</t>
-  </si>
-  <si>
     <t>Regular cubes</t>
   </si>
   <si>
     <t>Cubes</t>
   </si>
   <si>
-    <t>Regular squares</t>
+    <t>PStag scaling</t>
+  </si>
+  <si>
+    <t>Orange</t>
+  </si>
+  <si>
+    <t>Unstructured tetrahedra</t>
+  </si>
+  <si>
+    <t>Hexagons</t>
   </si>
   <si>
     <t>Non conforming cartesian checkerboard</t>
   </si>
   <si>
-    <t>Unstructured tetrahedra</t>
-  </si>
-  <si>
     <t>Orange, BC violated. PB with mesh ?</t>
+  </si>
+  <si>
+    <t>Regular checkerboard</t>
   </si>
 </sst>
 </file>
@@ -440,7 +467,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,23 +511,23 @@
       <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="n">
-        <v>2</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0.3045719312326941</v>
+      <c r="F2" t="n">
+        <v>-3.487620212460162e-09</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
       </c>
       <c r="H2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="I2" t="n">
+        <v>4.174916982650757</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -511,25 +538,25 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" t="n">
-        <v>2</v>
-      </c>
-      <c r="F3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0.4681105553490659</v>
+        <v>9</v>
+      </c>
+      <c r="D3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="n">
+        <v>-7.023350625076041e-06</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
       </c>
       <c r="H3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="I3" t="n">
+        <v>7.048214912414551</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -537,28 +564,28 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" t="n">
-        <v>2</v>
-      </c>
-      <c r="F4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" t="n">
-        <v>1.059914731644485</v>
+        <v>15</v>
+      </c>
+      <c r="D4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.4729127324588655</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
       </c>
       <c r="H4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I4" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="I4" t="n">
+        <v>2.912660837173462</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -569,25 +596,25 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" t="n">
-        <v>3</v>
-      </c>
-      <c r="F5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0.6676236238380446</v>
+        <v>9</v>
+      </c>
+      <c r="D5" t="n">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" t="n">
+        <v>-8.25752331143273e-11</v>
+      </c>
+      <c r="G5" t="s">
+        <v>18</v>
       </c>
       <c r="H5" t="s">
-        <v>21</v>
-      </c>
-      <c r="I5" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="I5" t="n">
+        <v>4.159222841262817</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -595,28 +622,28 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" t="n">
-        <v>2</v>
-      </c>
-      <c r="F6" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" t="n">
-        <v>1.004995658904568</v>
+        <v>19</v>
+      </c>
+      <c r="D6" t="n">
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.3045719312326941</v>
+      </c>
+      <c r="G6" t="s">
+        <v>21</v>
       </c>
       <c r="H6" t="s">
-        <v>17</v>
-      </c>
-      <c r="I6" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="I6" t="n">
+        <v>9.077556848526001</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -627,25 +654,25 @@
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" t="n">
-        <v>2</v>
-      </c>
-      <c r="F7" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7" t="n">
-        <v>0.1750269153763404</v>
+        <v>9</v>
+      </c>
+      <c r="D7" t="n">
+        <v>2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" t="n">
+        <v>-3.864405473494067e-05</v>
+      </c>
+      <c r="G7" t="s">
+        <v>13</v>
       </c>
       <c r="H7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I7" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="I7" t="n">
+        <v>6.195679187774658</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -656,25 +683,25 @@
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" t="n">
-        <v>2</v>
-      </c>
-      <c r="F8" t="s">
-        <v>18</v>
-      </c>
-      <c r="G8" t="n">
-        <v>0.3068899290492609</v>
+        <v>9</v>
+      </c>
+      <c r="D8" t="n">
+        <v>3</v>
+      </c>
+      <c r="E8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" t="n">
+        <v>-1.117834915917594e-11</v>
+      </c>
+      <c r="G8" t="s">
+        <v>24</v>
       </c>
       <c r="H8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I8" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="I8" t="n">
+        <v>77.44465613365173</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -682,28 +709,28 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" t="n">
-        <v>3</v>
-      </c>
-      <c r="F9" t="s">
-        <v>24</v>
-      </c>
-      <c r="G9" t="n">
-        <v>0.3293893511772948</v>
+        <v>15</v>
+      </c>
+      <c r="D9" t="n">
+        <v>2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.4681105553490659</v>
+      </c>
+      <c r="G9" t="s">
+        <v>13</v>
       </c>
       <c r="H9" t="s">
-        <v>12</v>
-      </c>
-      <c r="I9" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="I9" t="n">
+        <v>19.83197498321533</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -711,28 +738,28 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" t="n">
-        <v>3</v>
-      </c>
-      <c r="F10" t="s">
-        <v>24</v>
-      </c>
-      <c r="G10" t="n">
-        <v>0.2703534926287837</v>
+        <v>19</v>
+      </c>
+      <c r="D10" t="n">
+        <v>2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" t="n">
+        <v>1.059914731644485</v>
+      </c>
+      <c r="G10" t="s">
+        <v>18</v>
       </c>
       <c r="H10" t="s">
-        <v>12</v>
-      </c>
-      <c r="I10" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="I10" t="n">
+        <v>30.8527820110321</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -740,28 +767,314 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" t="n">
+        <v>3</v>
+      </c>
+      <c r="E11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.6676236238380446</v>
+      </c>
+      <c r="G11" t="s">
+        <v>27</v>
+      </c>
+      <c r="H11" t="s">
+        <v>11</v>
+      </c>
+      <c r="I11" t="n">
+        <v>24.40386915206909</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" t="n">
+        <v>2</v>
+      </c>
+      <c r="E12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" t="n">
+        <v>1.004995658904568</v>
+      </c>
+      <c r="G12" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" t="s">
+        <v>11</v>
+      </c>
+      <c r="I12" t="n">
+        <v>1.465689182281494</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
         <v>8</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" t="n">
+        <v>2</v>
+      </c>
+      <c r="E13" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" t="n">
+        <v>-0.0002403283177935742</v>
+      </c>
+      <c r="G13" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" t="s">
+        <v>11</v>
+      </c>
+      <c r="I13" t="n">
+        <v>49.10713601112366</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" t="n">
+        <v>3</v>
+      </c>
+      <c r="E14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" t="n">
+        <v>-3.26265785023925e-05</v>
+      </c>
+      <c r="G14" t="s">
+        <v>27</v>
+      </c>
+      <c r="H14" t="s">
+        <v>11</v>
+      </c>
+      <c r="I14" t="n">
+        <v>12.21128106117249</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
         <v>14</v>
       </c>
-      <c r="D11" t="s">
+      <c r="C15" t="s">
         <v>15</v>
       </c>
-      <c r="E11" t="n">
+      <c r="D15" t="n">
+        <v>2</v>
+      </c>
+      <c r="E15" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.3068899290492609</v>
+      </c>
+      <c r="G15" t="s">
+        <v>13</v>
+      </c>
+      <c r="H15" t="s">
+        <v>11</v>
+      </c>
+      <c r="I15" t="n">
+        <v>3.175358057022095</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" t="n">
+        <v>2</v>
+      </c>
+      <c r="E16" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" t="n">
+        <v>8.013761360562131e-05</v>
+      </c>
+      <c r="G16" t="s">
+        <v>18</v>
+      </c>
+      <c r="H16" t="s">
+        <v>29</v>
+      </c>
+      <c r="I16" t="n">
+        <v>143.7209329605103</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" t="n">
         <v>3</v>
       </c>
-      <c r="F11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G11" t="n">
+      <c r="E17" t="s">
+        <v>30</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.3293893511772948</v>
+      </c>
+      <c r="G17" t="s">
+        <v>24</v>
+      </c>
+      <c r="H17" t="s"/>
+      <c r="I17" t="s"/>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" t="n">
+        <v>2</v>
+      </c>
+      <c r="E18" t="s">
+        <v>16</v>
+      </c>
+      <c r="F18" t="n">
+        <v>-8.564714050813453e-06</v>
+      </c>
+      <c r="G18" t="s">
+        <v>31</v>
+      </c>
+      <c r="H18" t="s">
+        <v>11</v>
+      </c>
+      <c r="I18" t="n">
+        <v>7.83158802986145</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" t="n">
+        <v>3</v>
+      </c>
+      <c r="E19" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.2703534926287837</v>
+      </c>
+      <c r="G19" t="s">
+        <v>24</v>
+      </c>
+      <c r="H19" t="s">
+        <v>11</v>
+      </c>
+      <c r="I19" t="n">
+        <v>37.03536081314087</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" t="n">
+        <v>3</v>
+      </c>
+      <c r="E20" t="s">
+        <v>32</v>
+      </c>
+      <c r="F20" t="n">
         <v>-0.08672082382725707</v>
       </c>
-      <c r="H11" t="s">
-        <v>21</v>
-      </c>
-      <c r="I11" t="s">
-        <v>25</v>
+      <c r="G20" t="s">
+        <v>27</v>
+      </c>
+      <c r="H20" t="s">
+        <v>33</v>
+      </c>
+      <c r="I20" t="n">
+        <v>13.71957111358643</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" t="n">
+        <v>2</v>
+      </c>
+      <c r="E21" t="s">
+        <v>34</v>
+      </c>
+      <c r="F21" t="n">
+        <v>-1.855096236805034e-11</v>
+      </c>
+      <c r="G21" t="s">
+        <v>13</v>
+      </c>
+      <c r="H21" t="s">
+        <v>11</v>
+      </c>
+      <c r="I21" t="n">
+        <v>6.419693946838379</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the test synthesis notebook, html and tables
</commit_message>
<xml_diff>
--- a/tests/validation/test_synthesis/Convergence_table_short.xlsx
+++ b/tests/validation/test_synthesis/Convergence_table_short.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="35">
   <si>
     <t>PDE_model</t>
   </si>
@@ -40,91 +40,85 @@
     <t>Computational_time</t>
   </si>
   <si>
+    <t>Poisson</t>
+  </si>
+  <si>
+    <t>VF5</t>
+  </si>
+  <si>
+    <t>Deformed_quadrangles</t>
+  </si>
+  <si>
+    <t>Squares</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>Non_conforming_checkerboard</t>
+  </si>
+  <si>
+    <t>Non_conforming_locally_refined</t>
+  </si>
+  <si>
+    <t>Regular_brickwall</t>
+  </si>
+  <si>
+    <t>Regular_hexagons</t>
+  </si>
+  <si>
+    <t>Hexagons</t>
+  </si>
+  <si>
+    <t>Regular_squares</t>
+  </si>
+  <si>
+    <t>Unstructured_triangles</t>
+  </si>
+  <si>
+    <t>Triangles</t>
+  </si>
+  <si>
     <t>Wave system</t>
   </si>
   <si>
+    <t>PStag no scaling</t>
+  </si>
+  <si>
+    <t>Regular squares</t>
+  </si>
+  <si>
+    <t>Unstructured triangles</t>
+  </si>
+  <si>
+    <t>Orange</t>
+  </si>
+  <si>
     <t>Upwind</t>
   </si>
   <si>
     <t>Deformed quadrangles</t>
   </si>
   <si>
-    <t>Green</t>
-  </si>
-  <si>
-    <t>Poisson</t>
-  </si>
-  <si>
-    <t>VF5</t>
-  </si>
-  <si>
-    <t>Regular brickwall</t>
-  </si>
-  <si>
-    <t>Squares</t>
-  </si>
-  <si>
     <t>Regular brick wall</t>
   </si>
   <si>
+    <t>Regular checkerboard</t>
+  </si>
+  <si>
     <t>Regular hexagons</t>
   </si>
   <si>
-    <t>Hexagons</t>
-  </si>
-  <si>
-    <t>Unstructured triangles</t>
-  </si>
-  <si>
-    <t>Triangles</t>
-  </si>
-  <si>
-    <t>Poisson-Beltrami</t>
-  </si>
-  <si>
-    <t>P1 FE</t>
-  </si>
-  <si>
-    <t>Unstructured 3D triangles</t>
-  </si>
-  <si>
-    <t>3DTriangles</t>
-  </si>
-  <si>
-    <t>Regular squares</t>
+    <t>Regular cubes</t>
+  </si>
+  <si>
+    <t>Cubes</t>
   </si>
   <si>
     <t>Regular tetrahedra</t>
   </si>
   <si>
     <t>Tetrahedra</t>
-  </si>
-  <si>
-    <t>Non conforming cartesian locally refined</t>
-  </si>
-  <si>
-    <t>Regular cubes</t>
-  </si>
-  <si>
-    <t>Cubes</t>
-  </si>
-  <si>
-    <t>PStag scaling</t>
-  </si>
-  <si>
-    <t>Non conforming cartesian checkerboard</t>
-  </si>
-  <si>
-    <t>Orange</t>
-  </si>
-  <si>
-    <t>Unstructured tetrahedra</t>
-  </si>
-  <si>
-    <t>Orange, BC violated. PB with mesh ?</t>
-  </si>
-  <si>
-    <t>Regular checkerboard</t>
   </si>
 </sst>
 </file>
@@ -473,7 +467,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -509,7 +503,7 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="1" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
@@ -524,50 +518,50 @@
         <v>10</v>
       </c>
       <c r="F2" t="n">
-        <v>-3.487620212460162e-09</v>
+        <v>1.099715148758754</v>
       </c>
       <c r="G2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I2" t="n">
-        <v>3.828163862228394</v>
+        <v>8.325439929962158</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="1" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" t="n">
-        <v>2</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
       <c r="F3" t="n">
-        <v>0.2765875795876068</v>
+        <v>0.3500538307526435</v>
       </c>
       <c r="G3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="H3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I3" t="n">
-        <v>2.769896030426025</v>
+        <v>6.347608089447021</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="1" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
@@ -579,53 +573,53 @@
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F4" t="n">
-        <v>-7.023350625076041e-06</v>
+        <v>0.936221110698956</v>
       </c>
       <c r="G4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="H4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I4" t="n">
-        <v>6.772464036941528</v>
+        <v>19.86432003974915</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D5" t="n">
         <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F5" t="n">
-        <v>0.4809394106469453</v>
+        <v>-0.2073891905776415</v>
       </c>
       <c r="G5" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I5" t="n">
-        <v>3.251822948455811</v>
+        <v>2.677490949630737</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
@@ -637,53 +631,53 @@
         <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F6" t="n">
-        <v>-8.25752331143273e-11</v>
+        <v>1.94163703307054</v>
       </c>
       <c r="G6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="H6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I6" t="n">
-        <v>4.062403917312622</v>
+        <v>3.250871896743774</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="1" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="D7" t="n">
         <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="F7" t="n">
-        <v>0.3045719312326941</v>
+        <v>2.009991317810532</v>
       </c>
       <c r="G7" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="H7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I7" t="n">
-        <v>9.058223962783813</v>
+        <v>1.420461177825928</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="1" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
@@ -695,481 +689,309 @@
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="F8" t="n">
-        <v>-3.864405473494067e-05</v>
+        <v>0.6137798580984675</v>
       </c>
       <c r="G8" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="H8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I8" t="n">
-        <v>6.06682300567627</v>
+        <v>3.168046951293945</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="1" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="D9" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E9" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F9" t="n">
-        <v>-1.117834915917594e-11</v>
+        <v>-0.0002403281271210094</v>
       </c>
       <c r="G9" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="H9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I9" t="n">
-        <v>74.73377513885498</v>
+        <v>137.9682860374451</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="1" t="n">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="D10" t="n">
         <v>2</v>
       </c>
       <c r="E10" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F10" t="n">
-        <v>0.468110555349478</v>
+        <v>8.013775249613408e-05</v>
       </c>
       <c r="G10" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="H10" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="I10" t="n">
-        <v>21.61764097213745</v>
+        <v>388.8398141860962</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="1" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="D11" t="n">
         <v>2</v>
       </c>
       <c r="E11" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="F11" t="n">
-        <v>1.059914731644485</v>
+        <v>-3.487620212460162e-09</v>
       </c>
       <c r="G11" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="H11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I11" t="n">
-        <v>30.91114497184753</v>
+        <v>4.268468856811523</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="1" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="D12" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F12" t="n">
-        <v>0.6676236238380446</v>
+        <v>-7.023350625076041e-06</v>
       </c>
       <c r="G12" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="H12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I12" t="n">
-        <v>24.28290319442749</v>
+        <v>8.631521940231323</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" t="n">
+        <v>2</v>
+      </c>
+      <c r="E13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13" t="n">
+        <v>-1.855096236805034e-11</v>
+      </c>
+      <c r="G13" t="s">
         <v>11</v>
       </c>
-      <c r="B13" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" t="n">
-        <v>2</v>
-      </c>
-      <c r="E13" t="s">
-        <v>25</v>
-      </c>
-      <c r="F13" t="n">
-        <v>1.004995658905266</v>
-      </c>
-      <c r="G13" t="s">
-        <v>15</v>
-      </c>
       <c r="H13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I13" t="n">
-        <v>1.558310031890869</v>
+        <v>6.753997087478638</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="1" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D14" t="n">
         <v>2</v>
       </c>
       <c r="E14" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F14" t="n">
-        <v>-0.0002403283177935742</v>
+        <v>-8.564714050813453e-06</v>
       </c>
       <c r="G14" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H14" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I14" t="n">
-        <v>46.99151992797852</v>
+        <v>9.09241509437561</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="1" t="n">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B15" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C15" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="D15" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E15" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="F15" t="n">
-        <v>-3.26265785023925e-05</v>
+        <v>-3.864405473494067e-05</v>
       </c>
       <c r="G15" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="H15" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I15" t="n">
-        <v>11.38103103637695</v>
+        <v>6.354268789291382</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="1" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C16" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="D16" t="n">
         <v>2</v>
       </c>
       <c r="E16" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="F16" t="n">
-        <v>0.1750269153763217</v>
+        <v>-8.25752331143273e-11</v>
       </c>
       <c r="G16" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="H16" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I16" t="n">
-        <v>6.631990194320679</v>
+        <v>4.388073921203613</v>
       </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="1" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B17" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C17" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="D17" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E17" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="F17" t="n">
-        <v>0.3068899290492337</v>
+        <v>-3.26265785023925e-05</v>
       </c>
       <c r="G17" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="H17" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I17" t="n">
-        <v>3.162709951400757</v>
+        <v>13.37891101837158</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="1" t="n">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B18" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C18" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D18" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E18" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="F18" t="n">
-        <v>8.013761360562131e-05</v>
+        <v>-1.117834915917594e-11</v>
       </c>
       <c r="G18" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="H18" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="I18" t="n">
-        <v>138.8115110397339</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="A19" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="B19" t="s">
-        <v>12</v>
-      </c>
-      <c r="C19" t="s">
-        <v>22</v>
-      </c>
-      <c r="D19" t="n">
-        <v>3</v>
-      </c>
-      <c r="E19" t="s">
-        <v>34</v>
-      </c>
-      <c r="F19" t="n">
-        <v>0.3293893511772948</v>
-      </c>
-      <c r="G19" t="s">
-        <v>27</v>
-      </c>
-      <c r="H19" t="s">
-        <v>11</v>
-      </c>
-      <c r="I19" t="s"/>
-    </row>
-    <row r="20" spans="1:9">
-      <c r="A20" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="B20" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" t="s">
-        <v>9</v>
-      </c>
-      <c r="D20" t="n">
-        <v>2</v>
-      </c>
-      <c r="E20" t="s">
-        <v>17</v>
-      </c>
-      <c r="F20" t="n">
-        <v>-8.564714050813453e-06</v>
-      </c>
-      <c r="G20" t="s">
-        <v>18</v>
-      </c>
-      <c r="H20" t="s">
-        <v>11</v>
-      </c>
-      <c r="I20" t="n">
-        <v>7.626202821731567</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
-      <c r="A21" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="B21" t="s">
-        <v>12</v>
-      </c>
-      <c r="C21" t="s">
-        <v>13</v>
-      </c>
-      <c r="D21" t="n">
-        <v>3</v>
-      </c>
-      <c r="E21" t="s">
-        <v>34</v>
-      </c>
-      <c r="F21" t="n">
-        <v>0.2703534926287837</v>
-      </c>
-      <c r="G21" t="s">
-        <v>27</v>
-      </c>
-      <c r="H21" t="s">
-        <v>11</v>
-      </c>
-      <c r="I21" t="n">
-        <v>38.39829301834106</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
-      <c r="A22" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="B22" t="s">
-        <v>12</v>
-      </c>
-      <c r="C22" t="s">
-        <v>13</v>
-      </c>
-      <c r="D22" t="n">
-        <v>3</v>
-      </c>
-      <c r="E22" t="s">
-        <v>32</v>
-      </c>
-      <c r="F22" t="n">
-        <v>-0.08672082382725707</v>
-      </c>
-      <c r="G22" t="s">
-        <v>30</v>
-      </c>
-      <c r="H22" t="s">
-        <v>35</v>
-      </c>
-      <c r="I22" t="n">
-        <v>13.94595193862915</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9">
-      <c r="A23" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="B23" t="s">
-        <v>12</v>
-      </c>
-      <c r="C23" t="s">
-        <v>13</v>
-      </c>
-      <c r="D23" t="n">
-        <v>2</v>
-      </c>
-      <c r="E23" t="s">
-        <v>10</v>
-      </c>
-      <c r="F23" t="n">
-        <v>0.5498575743793769</v>
-      </c>
-      <c r="G23" t="s">
-        <v>15</v>
-      </c>
-      <c r="H23" t="s">
-        <v>11</v>
-      </c>
-      <c r="I23" t="n">
-        <v>8.833956003189087</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9">
-      <c r="A24" s="1" t="n">
-        <v>22</v>
-      </c>
-      <c r="B24" t="s">
-        <v>8</v>
-      </c>
-      <c r="C24" t="s">
-        <v>9</v>
-      </c>
-      <c r="D24" t="n">
-        <v>2</v>
-      </c>
-      <c r="E24" t="s">
-        <v>36</v>
-      </c>
-      <c r="F24" t="n">
-        <v>-1.855096236805034e-11</v>
-      </c>
-      <c r="G24" t="s">
-        <v>15</v>
-      </c>
-      <c r="H24" t="s">
-        <v>11</v>
-      </c>
-      <c r="I24" t="n">
-        <v>6.107317924499512</v>
+        <v>82.49833798408508</v>
       </c>
     </row>
   </sheetData>

</xml_diff>